<commit_message>
Processed tabs and figs
</commit_message>
<xml_diff>
--- a/dat/xlsxs/dat0cal.xlsx
+++ b/dat/xlsxs/dat0cal.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="45">
   <si>
     <t>CuSO$_4$浓度</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -133,15 +133,72 @@
   <si>
     <t>$\Delta B^*/B_0$测量值</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CuSO$_4$浓度</t>
+  </si>
+  <si>
+    <t>5\%</t>
+  </si>
+  <si>
+    <t>1\%</t>
+  </si>
+  <si>
+    <t>0.5\%</t>
+  </si>
+  <si>
+    <t>0.05\%</t>
+  </si>
+  <si>
+    <t>共振频率$f_0$/MHz</t>
+  </si>
+  <si>
+    <t>共振峰高$y_0$/V</t>
+  </si>
+  <si>
+    <t>第一尾波峰位置$x_1$/ms</t>
+  </si>
+  <si>
+    <t>第一尾波峰高$y_1$/V</t>
+  </si>
+  <si>
+    <t>第二尾波峰位置$x_2$/ms</t>
+  </si>
+  <si>
+    <t>第二尾波峰高$y_2$/V</t>
+  </si>
+  <si>
+    <t>第三尾波峰位置$x_3$/ms</t>
+  </si>
+  <si>
+    <t>第三尾波峰高$y_3$/V</t>
+  </si>
+  <si>
+    <t>第四尾波峰位置$x_4$/ms</t>
+  </si>
+  <si>
+    <t>第四尾波峰高$y_4$/V</t>
+  </si>
+  <si>
+    <t>尾波消失位置$x_0$/ms</t>
+  </si>
+  <si>
+    <t>表观横向弛豫时间$T^{*}_2$/ms</t>
+  </si>
+  <si>
+    <t>$\Delta B^*/B_0$测量值</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.000"/>
     <numFmt numFmtId="177" formatCode="0.0000"/>
+    <numFmt numFmtId="178" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="179" formatCode="0.000_);[Red]\(0.000\)"/>
+    <numFmt numFmtId="180" formatCode="0.0000_);[Red]\(0.0000\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -160,7 +217,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +233,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,7 +275,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -270,6 +333,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -285,6 +381,1839 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13349383485337712"/>
+          <c:y val="0.103074180804719"/>
+          <c:w val="0.8122588543338557"/>
+          <c:h val="0.76641576827689928"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>硫酸铜水溶液</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$21:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$13:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="0.0000">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-51F5-4F0A-9150-0AD898A1D34A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>纯水</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$23:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$24:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-51F5-4F0A-9150-0AD898A1D34A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2104491839"/>
+        <c:axId val="2104492671"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2104491839"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2104492671"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2104492671"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.9"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2104491839"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12693813453174471"/>
+          <c:y val="0.47757785442108991"/>
+          <c:w val="0.25933961492223545"/>
+          <c:h val="0.27600116351435455"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln cap="rnd">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:alpha val="90000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+          <a:ea typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$14:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6.4430321104833117E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5205237407751693E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.09741869239292E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1647602017161948E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.7270715319861307E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-383B-4873-9588-D346A2F89655}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="132889615"/>
+        <c:axId val="132886287"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="132889615"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="132886287"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="132886287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="132889615"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="图表 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -550,19 +2479,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -582,7 +2511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -602,207 +2531,207 @@
         <v>21.503</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="19">
         <v>4.08</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="19">
         <v>3.06</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="19">
         <v>2.5</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="19">
         <v>1.73</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="19">
         <v>0.42799999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="22">
         <v>0.78</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="22">
         <v>0.79</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="22">
         <v>0.81</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="22">
         <v>0.84</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="22">
         <v>0.87</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="19">
         <v>1.98</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="19">
         <v>1.77</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="19">
         <v>1.56</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="19">
         <v>1.1100000000000001</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="19">
         <v>0.224</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="21">
         <v>1.26</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="21">
         <v>1.27</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="21">
         <v>1.3</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="21">
         <v>1.33</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="21">
         <v>1.36</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="20">
         <v>0.96</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="19">
         <v>1.02</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="19">
         <v>0.9</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="19">
         <v>0.65</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="19">
         <v>0.126</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="21">
         <v>1.66</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="21">
         <v>1.66</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="21">
         <v>1.69</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="21">
         <v>1.72</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="21">
         <v>1.74</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="20">
         <v>0.48</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="20">
         <v>0.6</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="20">
         <v>0.54</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="20">
         <v>0.39</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="23">
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="21">
         <v>2</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="21">
         <v>1.99</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="21">
         <v>2.0299999999999998</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="21">
         <v>2.0499999999999998</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="21">
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="20">
         <v>0.24</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="20">
         <v>0.37</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="20">
         <v>0.35</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="20">
         <v>0.27</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="23">
         <v>0.08</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="21">
         <v>3.55</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="21">
         <v>3.33</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="21">
         <v>3.32</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="21">
         <v>3.57</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="21">
         <v>3.84</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -822,43 +2751,375 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="24">
         <f>Sheet2!B10</f>
         <v>6.4430321104833117E-5</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="24">
         <f>Sheet2!B21</f>
         <v>4.5205237407751693E-5</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="24">
         <f>Sheet2!B35</f>
         <v>4.09741869239292E-5</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="24">
         <f>Sheet2!B49</f>
         <v>4.1647602017161948E-5</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="24">
         <f>Sheet2!B63</f>
         <v>4.7270715319861307E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f>AVERAGE(B14:F14)</f>
+        <v>4.7905612554707454E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="B16">
         <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f>0.05</f>
+        <v>0.05</v>
+      </c>
+      <c r="C21">
+        <f>0.01</f>
+        <v>0.01</v>
+      </c>
+      <c r="D21">
+        <f>0.005</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E21">
+        <f>0.0005</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="F21">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <f>F13</f>
+        <v>1.29</v>
+      </c>
+      <c r="C24" s="1">
+        <f>F13</f>
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="28">
+        <v>21.512</v>
+      </c>
+      <c r="C27" s="28">
+        <v>21.509</v>
+      </c>
+      <c r="D27" s="28">
+        <v>21.507000000000001</v>
+      </c>
+      <c r="E27" s="28">
+        <v>21.504000000000001</v>
+      </c>
+      <c r="F27" s="28">
+        <v>21.503</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="28">
+        <v>4.08</v>
+      </c>
+      <c r="C28" s="28">
+        <v>3.06</v>
+      </c>
+      <c r="D28" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="E28" s="28">
+        <v>1.73</v>
+      </c>
+      <c r="F28" s="28">
+        <v>0.42799999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="28">
+        <v>0.78</v>
+      </c>
+      <c r="C29" s="28">
+        <v>0.79</v>
+      </c>
+      <c r="D29" s="28">
+        <v>0.81</v>
+      </c>
+      <c r="E29" s="28">
+        <v>0.84</v>
+      </c>
+      <c r="F29" s="28">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="28">
+        <v>1.98</v>
+      </c>
+      <c r="C30" s="28">
+        <v>1.77</v>
+      </c>
+      <c r="D30" s="28">
+        <v>1.56</v>
+      </c>
+      <c r="E30" s="28">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F30" s="28">
+        <v>0.224</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="28">
+        <v>1.26</v>
+      </c>
+      <c r="C31" s="28">
+        <v>1.27</v>
+      </c>
+      <c r="D31" s="28">
+        <v>1.3</v>
+      </c>
+      <c r="E31" s="28">
+        <v>1.33</v>
+      </c>
+      <c r="F31" s="28">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="C32" s="28">
+        <v>1.02</v>
+      </c>
+      <c r="D32" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="E32" s="28">
+        <v>0.65</v>
+      </c>
+      <c r="F32" s="28">
+        <v>0.126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="28">
+        <v>1.66</v>
+      </c>
+      <c r="C33" s="28">
+        <v>1.66</v>
+      </c>
+      <c r="D33" s="28">
+        <v>1.69</v>
+      </c>
+      <c r="E33" s="28">
+        <v>1.72</v>
+      </c>
+      <c r="F33" s="28">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="28">
+        <v>0.48</v>
+      </c>
+      <c r="C34" s="28">
+        <v>0.6</v>
+      </c>
+      <c r="D34" s="28">
+        <v>0.54</v>
+      </c>
+      <c r="E34" s="28">
+        <v>0.39</v>
+      </c>
+      <c r="F34" s="28">
+        <v>7.5999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="28">
+        <v>2</v>
+      </c>
+      <c r="C35" s="28">
+        <v>1.99</v>
+      </c>
+      <c r="D35" s="28">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="E35" s="28">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="F35" s="28">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="28">
+        <v>0.24</v>
+      </c>
+      <c r="C36" s="28">
+        <v>0.37</v>
+      </c>
+      <c r="D36" s="28">
+        <v>0.35</v>
+      </c>
+      <c r="E36" s="28">
+        <v>0.27</v>
+      </c>
+      <c r="F36" s="28">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="28">
+        <v>3.55</v>
+      </c>
+      <c r="C37" s="28">
+        <v>3.33</v>
+      </c>
+      <c r="D37" s="28">
+        <v>3.32</v>
+      </c>
+      <c r="E37" s="28">
+        <v>3.57</v>
+      </c>
+      <c r="F37" s="28">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="28">
+        <v>0.99</v>
+      </c>
+      <c r="C38" s="28">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D38" s="28">
+        <v>1.31</v>
+      </c>
+      <c r="E38" s="28">
+        <v>1.35</v>
+      </c>
+      <c r="F38" s="28">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="29" t="str">
+        <f>TEXT(B14*100000,"0.00")&amp;"$\times 10^{-5}$"</f>
+        <v>6.44$\times 10^{-5}$</v>
+      </c>
+      <c r="C39" s="29" t="str">
+        <f t="shared" ref="C39:F39" si="0">TEXT(C14*100000,"0.00")&amp;"$\times 10^{-5}$"</f>
+        <v>4.52$\times 10^{-5}$</v>
+      </c>
+      <c r="D39" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>4.10$\times 10^{-5}$</v>
+      </c>
+      <c r="E39" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>4.16$\times 10^{-5}$</v>
+      </c>
+      <c r="F39" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>4.73$\times 10^{-5}$</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -866,8 +3127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -973,7 +3234,7 @@
         <v>0.7230001437096264</v>
       </c>
       <c r="D8" s="16">
-        <f t="shared" ref="D8:F9" si="0">LN($B6/D6)</f>
+        <f t="shared" ref="D8:F8" si="0">LN($B6/D6)</f>
         <v>1.4469189829363254</v>
       </c>
       <c r="E8" s="16">

</xml_diff>

<commit_message>
add Initial spike figs
</commit_message>
<xml_diff>
--- a/dat/xlsxs/dat0cal.xlsx
+++ b/dat/xlsxs/dat0cal.xlsx
@@ -1039,6 +1039,360 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14948104508519169"/>
+          <c:y val="0.13980499338409144"/>
+          <c:w val="0.8122588543338557"/>
+          <c:h val="0.76641576827689928"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>硫酸铜水溶液</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$21:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.08</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.73</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42799999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-26A3-4234-90DD-8197B47E65D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>纯水</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$23:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$25:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.42799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.42799999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-26A3-4234-90DD-8197B47E65D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2104491839"/>
+        <c:axId val="2104492671"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2104491839"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2104492671"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2104492671"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2104491839"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13093493708969833"/>
+          <c:y val="0.20668712898490996"/>
+          <c:w val="0.25933961492223545"/>
+          <c:h val="0.27600116351435455"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln cap="rnd">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:alpha val="90000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+          <a:ea typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Unicode Symbols" panose="05020102010707070707" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1119,6 +1473,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1636,6 +2030,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2208,6 +3118,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="图表 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2481,8 +3423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2828,6 +3770,16 @@
       <c r="C24" s="1">
         <f>F13</f>
         <v>1.29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="19">
+        <f>F3</f>
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="C25" s="19">
+        <f>F3</f>
+        <v>0.42799999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>